<commit_message>
Small script changes to change which tag the reader looks for
</commit_message>
<xml_diff>
--- a/Assignment_1/Bug statistics data.xlsx
+++ b/Assignment_1/Bug statistics data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\4313\Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2727761F-DC92-40B7-8B16-D2B08AB1F29A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52451D0D-ED2E-4894-8FA0-905044714B85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{7F720C22-5553-422E-9423-B9D6422B2769}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Bugs</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Cannot Reproduce</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Patch Avaliable</t>
   </si>
 </sst>
 </file>
@@ -243,7 +255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49D46515-8B7F-4736-B69F-6E11F1F9E699}" type="CELLRANGE">
+                    <a:fld id="{583D5B49-1CE9-4DD3-BFF9-DC376E5AF88B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -252,7 +264,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{1532D63F-E2D2-429A-B660-DABE74A5381F}" type="PERCENTAGE">
+                    <a:fld id="{4B3EF7BA-DBEA-46D5-8511-3CF25AE92F13}" type="PERCENTAGE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -286,7 +298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F012868-82D6-49A5-8059-76737298D54F}" type="CELLRANGE">
+                    <a:fld id="{B5290630-0F95-4BD5-A60B-01A4C9B68F41}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -295,7 +307,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{31C7F227-0A03-4658-B4FC-A3893EA85ECF}" type="PERCENTAGE">
+                    <a:fld id="{193692B3-54B5-4CB2-9FC2-F55972E18E5A}" type="PERCENTAGE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -545,7 +557,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -558,8 +570,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Current Status of Bug reports </a:t>
+              <a:rPr lang="en-CA"/>
+              <a:t>Bug Status Breakdown</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -577,7 +589,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -601,26 +613,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$24:$E$24</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Duplicate</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Fixed</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unresolved</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Invalid</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -628,26 +620,13 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-8655-4FA9-A140-1A6EA53C95EA}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -656,26 +635,13 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-8655-4FA9-A140-1A6EA53C95EA}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -684,26 +650,13 @@
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-8655-4FA9-A140-1A6EA53C95EA}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -712,232 +665,30 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-8655-4FA9-A140-1A6EA53C95EA}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.1129921259842621E-2"/>
-                  <c:y val="8.3311096529600462E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:noAutofit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="9.7652887139107608E-2"/>
-                      <c:h val="6.0115923009623796E-2"/>
-                    </c:manualLayout>
-                  </c15:layout>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-8655-4FA9-A140-1A6EA53C95EA}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.16315135608048995"/>
-                  <c:y val="-0.10019211140274133"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-8655-4FA9-A140-1A6EA53C95EA}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.11224956255468066"/>
-                  <c:y val="0.13763961796442112"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-8655-4FA9-A140-1A6EA53C95EA}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="4.1454068241469813E-2"/>
-                  <c:y val="0.12231517935258093"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-8655-4FA9-A140-1A6EA53C95EA}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$18:$J$18</c:f>
+              <c:f>Sheet1!$B$24:$E$24</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Duplicate</c:v>
+                  <c:v>Closed</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Fixed</c:v>
+                  <c:v>Open</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Unresolved</c:v>
+                  <c:v>Resolved</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Later</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Won't Fix</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Invalid</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Incomplete</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Not A Problem</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Cannot Reproduce</c:v>
+                  <c:v>Patch Avaliable</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -949,30 +700,29 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>454</c:v>
+                  <c:v>5138</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6101</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1419</c:v>
+                  <c:v>2615</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>640</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8655-4FA9-A140-1A6EA53C95EA}"/>
+              <c16:uniqueId val="{00000000-A2BA-47D8-AF77-ECCD5C96012F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -990,7 +740,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1664,7 +1414,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1675,7 +1425,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1687,6 +1437,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -1717,9 +1478,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1751,7 +1515,7 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1759,24 +1523,16 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:scene3d>
-        <a:camera prst="orthographicFront"/>
-        <a:lightRig rig="brightRoom" dir="t"/>
-      </a:scene3d>
-      <a:sp3d prstMaterial="flat">
-        <a:bevelT w="50800" h="101600" prst="angle"/>
-        <a:contourClr>
-          <a:srgbClr val="000000"/>
-        </a:contourClr>
-      </a:sp3d>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1784,10 +1540,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="19050">
+      <a:ln w="25400">
         <a:solidFill>
           <a:schemeClr val="lt1"/>
         </a:solidFill>
@@ -1813,8 +1566,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1822,17 +1577,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -2097,7 +1849,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2113,7 +1865,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2220,23 +1972,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>52386</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>461962</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C3DB9B9-345B-40AE-A6B3-081DCB266779}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4503B822-5AB8-4425-A6A7-9557F38C1F06}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2557,7 +2309,7 @@
   <dimension ref="B3:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:E25"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,30 +2393,30 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>454</v>
+        <v>5138</v>
       </c>
       <c r="C25">
-        <v>6101</v>
+        <v>691</v>
       </c>
       <c r="D25">
-        <v>1419</v>
+        <v>2615</v>
       </c>
       <c r="E25">
-        <v>640</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>